<commit_message>
Added analysis and also trendlines for graphs
</commit_message>
<xml_diff>
--- a/Results/Timings.xlsx
+++ b/Results/Timings.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Question 4" sheetId="1" r:id="rId1"/>
@@ -342,11 +342,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="56782208"/>
-        <c:axId val="56780672"/>
+        <c:axId val="125460864"/>
+        <c:axId val="125462784"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="56782208"/>
+        <c:axId val="125460864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -380,12 +380,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56780672"/>
+        <c:crossAx val="125462784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="56780672"/>
+        <c:axId val="125462784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -415,7 +415,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56782208"/>
+        <c:crossAx val="125460864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -486,6 +486,20 @@
           <c:tx>
             <c:v>Question 6 Greedy  Timings</c:v>
           </c:tx>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.25711701662292213"/>
+                  <c:y val="-0.16870844269466317"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Question6!$A$3:$A$102</c:f>
@@ -1114,11 +1128,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="143018624"/>
-        <c:axId val="143020800"/>
+        <c:axId val="138038656"/>
+        <c:axId val="138044928"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="143018624"/>
+        <c:axId val="138038656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1152,12 +1166,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="143020800"/>
+        <c:crossAx val="138044928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="143020800"/>
+        <c:axId val="138044928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1187,7 +1201,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="143018624"/>
+        <c:crossAx val="138038656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1258,6 +1272,20 @@
           <c:tx>
             <c:v>Question 6 Dynamic  Timings</c:v>
           </c:tx>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.14833092738407699"/>
+                  <c:y val="-0.17201334208223973"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Question6!$D$3:$D$32</c:f>
@@ -1466,11 +1494,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="137312512"/>
-        <c:axId val="139444608"/>
+        <c:axId val="138061312"/>
+        <c:axId val="138063232"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="137312512"/>
+        <c:axId val="138061312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1504,12 +1532,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="139444608"/>
+        <c:crossAx val="138063232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="139444608"/>
+        <c:axId val="138063232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1539,7 +1567,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137312512"/>
+        <c:crossAx val="138061312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1906,11 +1934,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="137357184"/>
-        <c:axId val="143736832"/>
+        <c:axId val="138121600"/>
+        <c:axId val="138123520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="137357184"/>
+        <c:axId val="138121600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1944,12 +1972,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="143736832"/>
+        <c:crossAx val="138123520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="143736832"/>
+        <c:axId val="138123520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1979,7 +2007,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137357184"/>
+        <c:crossAx val="138121600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2041,6 +2069,20 @@
           <c:tx>
             <c:v>Question 4 Greedy</c:v>
           </c:tx>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.32397834645669293"/>
+                  <c:y val="-8.8322032662583844E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>'Question 4'!$G$3:$G$102</c:f>
@@ -2663,11 +2705,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="60183680"/>
-        <c:axId val="60185984"/>
+        <c:axId val="125483264"/>
+        <c:axId val="125497728"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="60183680"/>
+        <c:axId val="125483264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2701,12 +2743,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60185984"/>
+        <c:crossAx val="125497728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="60185984"/>
+        <c:axId val="125497728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2736,7 +2778,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60183680"/>
+        <c:crossAx val="125483264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2798,6 +2840,20 @@
           <c:tx>
             <c:v>Question 4 Dynamic Timings</c:v>
           </c:tx>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.15998381452318461"/>
+                  <c:y val="-0.129776538349373"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>'Question 4'!$D$3:$D$32</c:f>
@@ -3006,11 +3062,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="59853056"/>
-        <c:axId val="59945728"/>
+        <c:axId val="125781888"/>
+        <c:axId val="125784064"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="59853056"/>
+        <c:axId val="125781888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3044,12 +3100,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59945728"/>
+        <c:crossAx val="125784064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="59945728"/>
+        <c:axId val="125784064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3079,7 +3135,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59853056"/>
+        <c:crossAx val="125781888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3150,6 +3206,20 @@
           <c:tx>
             <c:v>Question 5A Greedy Timings</c:v>
           </c:tx>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.30175612423447068"/>
+                  <c:y val="-0.12525371828521434"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>'Question 5A'!$A$3:$A$102</c:f>
@@ -3778,11 +3848,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="77129216"/>
-        <c:axId val="113125248"/>
+        <c:axId val="137856512"/>
+        <c:axId val="137858432"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="77129216"/>
+        <c:axId val="137856512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3816,12 +3886,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113125248"/>
+        <c:crossAx val="137858432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="113125248"/>
+        <c:axId val="137858432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3851,7 +3921,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77129216"/>
+        <c:crossAx val="137856512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3922,6 +3992,20 @@
           <c:tx>
             <c:v>Question 5A Dynamic timings</c:v>
           </c:tx>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="3.7761592300962377E-2"/>
+                  <c:y val="-0.18234106153397492"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>'Question 5A'!$D$3:$D$32</c:f>
@@ -4130,11 +4214,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="73226112"/>
-        <c:axId val="77073024"/>
+        <c:axId val="137883648"/>
+        <c:axId val="137885568"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="73226112"/>
+        <c:axId val="137883648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4168,12 +4252,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77073024"/>
+        <c:crossAx val="137885568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="77073024"/>
+        <c:axId val="137885568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4203,7 +4287,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73226112"/>
+        <c:crossAx val="137883648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4566,11 +4650,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="124750464"/>
-        <c:axId val="136063232"/>
+        <c:axId val="138173056"/>
+        <c:axId val="138179328"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="124750464"/>
+        <c:axId val="138173056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4604,12 +4688,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="136063232"/>
+        <c:crossAx val="138179328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="136063232"/>
+        <c:axId val="138179328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4639,7 +4723,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124750464"/>
+        <c:crossAx val="138173056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4710,6 +4794,20 @@
           <c:tx>
             <c:v>Question 5B Greedy Timings</c:v>
           </c:tx>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.30475612423447068"/>
+                  <c:y val="-0.21854367162438029"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Question5b!$A$3:$A$102</c:f>
@@ -5338,11 +5436,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="124805504"/>
-        <c:axId val="134664960"/>
+        <c:axId val="127543168"/>
+        <c:axId val="127553536"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="124805504"/>
+        <c:axId val="127543168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5376,12 +5474,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134664960"/>
+        <c:crossAx val="127553536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="134664960"/>
+        <c:axId val="127553536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5411,7 +5509,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124805504"/>
+        <c:crossAx val="127543168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5482,6 +5580,20 @@
           <c:tx>
             <c:v>Question 5B Dynamic  Timings</c:v>
           </c:tx>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.12942825896762905"/>
+                  <c:y val="-0.14839129483814523"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Question5b!$D$3:$D$32</c:f>
@@ -5690,11 +5802,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="124802944"/>
-        <c:axId val="134479232"/>
+        <c:axId val="127590400"/>
+        <c:axId val="127592320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="124802944"/>
+        <c:axId val="127590400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5728,12 +5840,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134479232"/>
+        <c:crossAx val="127592320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="134479232"/>
+        <c:axId val="127592320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5763,7 +5875,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124802944"/>
+        <c:crossAx val="127590400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6312,11 +6424,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="91497984"/>
-        <c:axId val="91499904"/>
+        <c:axId val="127700992"/>
+        <c:axId val="127702912"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="91497984"/>
+        <c:axId val="127700992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6350,12 +6462,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91499904"/>
+        <c:crossAx val="127702912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="91499904"/>
+        <c:axId val="127702912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6385,7 +6497,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91497984"/>
+        <c:crossAx val="127700992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6406,16 +6518,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6436,16 +6548,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6468,15 +6580,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -6805,51 +6917,51 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Quest4timings" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Quest6timings" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Quest6timings_1" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Quest8change" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Quest9change_1" connectionId="12" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Quest6timings_1" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Quest8change" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Quest6timings" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Quest4timings_1" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Quest4timings" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Quest5atimings" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Quest5Atimings_1" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Quest10change" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Quest5atimings" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Quest5Btimings" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Quest5Btimings_1" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Quest11change" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Quest5Btimings" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7141,7 +7253,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="G4" workbookViewId="0">
       <selection activeCell="V12" sqref="V12"/>
     </sheetView>
   </sheetViews>
@@ -8239,7 +8351,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="E4" workbookViewId="0">
       <selection activeCell="U19" sqref="U19"/>
     </sheetView>
   </sheetViews>
@@ -9537,7 +9649,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H102"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="R19" sqref="R19"/>
     </sheetView>
   </sheetViews>
@@ -11019,8 +11131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H102"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="N53" sqref="N53"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>